<commit_message>
Atualização automática [Thu Jul 24 03:04:32 UTC 2025]
</commit_message>
<xml_diff>
--- a/livelo_parceiros.xlsx
+++ b/livelo_parceiros.xlsx
@@ -468,7 +468,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -496,12 +496,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Azul Viagens</t>
+          <t>Localiza</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -511,25 +511,25 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>R$</t>
+          <t>U$</t>
         </is>
       </c>
       <c r="E3" t="n">
         <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Localiza</t>
+          <t>ABC da Construcao</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -539,25 +539,25 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>U$</t>
+          <t>R$</t>
         </is>
       </c>
       <c r="E4" t="n">
         <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ABC da Construcao</t>
+          <t>PerfectDraft (Ambev)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -574,23 +574,23 @@
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>PerfectDraft (Ambev)</t>
+          <t>ASICS</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -602,18 +602,18 @@
         <v>1</v>
       </c>
       <c r="F6" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ASICS</t>
+          <t>Angeloni</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -636,17 +636,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Angeloni</t>
+          <t>Divvino</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -658,23 +658,23 @@
         <v>1</v>
       </c>
       <c r="F8" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Divvino</t>
+          <t>Cruzeiros Agaxtur</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -686,74 +686,74 @@
         <v>1</v>
       </c>
       <c r="F9" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Cruzeiros Agaxtur</t>
+          <t>Aliexpress</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>R$</t>
+          <t>U$</t>
         </is>
       </c>
       <c r="E10" t="n">
         <v>1</v>
       </c>
       <c r="F10" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Aliexpress</t>
+          <t>Trocafy</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>U$</t>
+          <t>R$</t>
         </is>
       </c>
       <c r="E11" t="n">
         <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Trocafy</t>
+          <t>Havaianas</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -776,12 +776,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Havaianas</t>
+          <t>Allianz</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -798,18 +798,18 @@
         <v>1</v>
       </c>
       <c r="F13" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Allianz</t>
+          <t>AMOBELEZA</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -826,18 +826,18 @@
         <v>1</v>
       </c>
       <c r="F14" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>AMOBELEZA</t>
+          <t>Tia Sônia</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -860,12 +860,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Tia Sônia</t>
+          <t>Amazon</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -888,12 +888,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Amazon</t>
+          <t>Aramis</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -910,23 +910,23 @@
         <v>1</v>
       </c>
       <c r="F17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Aramis</t>
+          <t>Assist Card Seguros</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -938,18 +938,18 @@
         <v>1</v>
       </c>
       <c r="F18" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Assist Card Seguros</t>
+          <t>Universal Assistance – Seguro Viagem</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -972,12 +972,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Universal Assistance – Seguro Viagem</t>
+          <t>Azul Viagens</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -994,13 +994,13 @@
         <v>1</v>
       </c>
       <c r="F20" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1056,7 +1056,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1084,7 +1084,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1112,7 +1112,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1140,7 +1140,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1168,7 +1168,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1196,7 +1196,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1224,7 +1224,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1252,7 +1252,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1280,7 +1280,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1308,7 +1308,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1336,7 +1336,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1364,7 +1364,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1392,7 +1392,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1420,7 +1420,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1476,7 +1476,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1504,7 +1504,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1532,7 +1532,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1560,7 +1560,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1588,7 +1588,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1616,7 +1616,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1644,7 +1644,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1672,7 +1672,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1700,7 +1700,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1728,7 +1728,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1756,7 +1756,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1784,7 +1784,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1812,7 +1812,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1840,7 +1840,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1896,7 +1896,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1924,7 +1924,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1952,7 +1952,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1980,7 +1980,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -2008,7 +2008,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -2036,7 +2036,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -2064,7 +2064,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -2092,7 +2092,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -2120,7 +2120,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -2148,7 +2148,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -2176,7 +2176,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -2204,7 +2204,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -2232,7 +2232,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -2260,7 +2260,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2316,7 +2316,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -2344,7 +2344,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -2372,7 +2372,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -2400,7 +2400,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2428,7 +2428,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2456,7 +2456,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2484,7 +2484,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -2512,7 +2512,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2540,7 +2540,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2568,7 +2568,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2596,7 +2596,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2624,7 +2624,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2652,7 +2652,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2680,7 +2680,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -2736,7 +2736,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -2764,7 +2764,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -2792,7 +2792,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2820,7 +2820,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2848,7 +2848,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -2876,7 +2876,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2904,7 +2904,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2932,7 +2932,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -2960,7 +2960,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -2988,7 +2988,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -3016,7 +3016,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -3044,7 +3044,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -3072,7 +3072,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -3100,7 +3100,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -3156,7 +3156,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -3184,7 +3184,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -3212,7 +3212,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -3240,7 +3240,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -3268,7 +3268,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -3296,7 +3296,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -3324,7 +3324,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -3352,7 +3352,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -3380,7 +3380,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -3408,7 +3408,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -3436,7 +3436,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -3464,7 +3464,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -3492,7 +3492,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -3520,7 +3520,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -3548,7 +3548,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3576,7 +3576,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3604,7 +3604,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -3632,7 +3632,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -3660,7 +3660,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
@@ -3670,7 +3670,7 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
@@ -3682,13 +3682,13 @@
         <v>1</v>
       </c>
       <c r="F116" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -3716,7 +3716,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -3744,7 +3744,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -3772,7 +3772,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -3800,7 +3800,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -3828,7 +3828,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -3856,7 +3856,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -3884,7 +3884,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -3912,7 +3912,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -3940,7 +3940,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -3968,7 +3968,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -3996,7 +3996,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -4024,7 +4024,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -4052,7 +4052,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -4080,7 +4080,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -4108,7 +4108,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -4136,7 +4136,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -4164,7 +4164,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -4192,7 +4192,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -4220,7 +4220,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -4248,7 +4248,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -4276,7 +4276,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -4304,7 +4304,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
@@ -4332,7 +4332,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -4360,7 +4360,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -4388,7 +4388,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -4416,7 +4416,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -4444,7 +4444,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -4472,7 +4472,7 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
@@ -4500,7 +4500,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
@@ -4528,7 +4528,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -4556,7 +4556,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -4584,7 +4584,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
@@ -4612,7 +4612,7 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
@@ -4640,7 +4640,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -4668,7 +4668,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -4696,7 +4696,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -4724,7 +4724,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -4752,7 +4752,7 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
@@ -4780,7 +4780,7 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
@@ -4808,7 +4808,7 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
@@ -4836,7 +4836,7 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
@@ -4864,7 +4864,7 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
@@ -4892,7 +4892,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -4920,7 +4920,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -4948,7 +4948,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -4976,7 +4976,7 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
@@ -5004,7 +5004,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
@@ -5032,7 +5032,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -5060,7 +5060,7 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
@@ -5088,7 +5088,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
@@ -5116,7 +5116,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
@@ -5144,7 +5144,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
@@ -5172,7 +5172,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
@@ -5200,7 +5200,7 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
@@ -5228,7 +5228,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
@@ -5256,7 +5256,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
@@ -5284,7 +5284,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -5312,7 +5312,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -5340,7 +5340,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -5368,7 +5368,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -5396,7 +5396,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -5424,7 +5424,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
@@ -5452,7 +5452,7 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
@@ -5480,7 +5480,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
@@ -5508,7 +5508,7 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
@@ -5536,7 +5536,7 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
@@ -5564,7 +5564,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
@@ -5592,7 +5592,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
@@ -5620,7 +5620,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -5648,7 +5648,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5676,7 +5676,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5704,7 +5704,7 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
@@ -5732,7 +5732,7 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
@@ -5760,7 +5760,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
@@ -5788,7 +5788,7 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
@@ -5816,7 +5816,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
@@ -5844,7 +5844,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -5872,7 +5872,7 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
@@ -5900,7 +5900,7 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
@@ -5928,7 +5928,7 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
@@ -5956,7 +5956,7 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
@@ -5984,7 +5984,7 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
@@ -6012,7 +6012,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
@@ -6040,7 +6040,7 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
@@ -6068,7 +6068,7 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
@@ -6096,7 +6096,7 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
@@ -6124,7 +6124,7 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
@@ -6152,7 +6152,7 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
@@ -6180,7 +6180,7 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
@@ -6208,7 +6208,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
@@ -6236,7 +6236,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -6264,7 +6264,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
@@ -6292,7 +6292,7 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
@@ -6320,7 +6320,7 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
@@ -6348,7 +6348,7 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
@@ -6376,7 +6376,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
@@ -6404,7 +6404,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
@@ -6432,7 +6432,7 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
@@ -6460,7 +6460,7 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
@@ -6488,7 +6488,7 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
@@ -6516,7 +6516,7 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
@@ -6544,7 +6544,7 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
@@ -6572,7 +6572,7 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
@@ -6600,7 +6600,7 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
@@ -6628,7 +6628,7 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
@@ -6656,7 +6656,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
@@ -6684,7 +6684,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
@@ -6712,7 +6712,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
@@ -6740,7 +6740,7 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
@@ -6768,7 +6768,7 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
@@ -6796,7 +6796,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
@@ -6824,7 +6824,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -6852,7 +6852,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -6880,7 +6880,7 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
@@ -6908,7 +6908,7 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
@@ -6936,7 +6936,7 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
@@ -6964,7 +6964,7 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
@@ -6992,7 +6992,7 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
@@ -7020,7 +7020,7 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
@@ -7048,7 +7048,7 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
@@ -7076,7 +7076,7 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
@@ -7104,7 +7104,7 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
@@ -7132,7 +7132,7 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
@@ -7160,7 +7160,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -7188,7 +7188,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
@@ -7216,7 +7216,7 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
@@ -7244,7 +7244,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
@@ -7272,7 +7272,7 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
@@ -7300,7 +7300,7 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
@@ -7328,7 +7328,7 @@
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
@@ -7356,7 +7356,7 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
@@ -7384,7 +7384,7 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
@@ -7412,7 +7412,7 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
@@ -7440,7 +7440,7 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
@@ -7468,7 +7468,7 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
@@ -7496,7 +7496,7 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
@@ -7524,7 +7524,7 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
@@ -7552,7 +7552,7 @@
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
@@ -7580,7 +7580,7 @@
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
@@ -7608,7 +7608,7 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
@@ -7636,7 +7636,7 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
@@ -7664,7 +7664,7 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
@@ -7692,7 +7692,7 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>2025-07-24 02:06:45</t>
+          <t>2025-07-24 03:04:11</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">

</xml_diff>

<commit_message>
Atualização automática [Thu Jul 24 03:52:32 UTC 2025]
</commit_message>
<xml_diff>
--- a/livelo_parceiros.xlsx
+++ b/livelo_parceiros.xlsx
@@ -468,7 +468,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -496,7 +496,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -524,7 +524,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -534,7 +534,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -546,13 +546,13 @@
         <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -580,7 +580,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -636,7 +636,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -664,7 +664,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -692,7 +692,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -720,7 +720,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -748,7 +748,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -776,7 +776,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -804,7 +804,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -832,7 +832,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -860,7 +860,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -888,7 +888,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -916,7 +916,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -944,7 +944,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -966,13 +966,13 @@
         <v>1</v>
       </c>
       <c r="F19" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -982,7 +982,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -994,13 +994,13 @@
         <v>1</v>
       </c>
       <c r="F20" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1010,7 +1010,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1022,13 +1022,13 @@
         <v>1</v>
       </c>
       <c r="F21" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1056,7 +1056,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1078,13 +1078,13 @@
         <v>1</v>
       </c>
       <c r="F23" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1094,7 +1094,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1106,13 +1106,13 @@
         <v>1</v>
       </c>
       <c r="F24" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1140,7 +1140,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1168,7 +1168,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1178,7 +1178,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1190,13 +1190,13 @@
         <v>1</v>
       </c>
       <c r="F27" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1224,7 +1224,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1234,7 +1234,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1246,13 +1246,13 @@
         <v>1</v>
       </c>
       <c r="F29" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1280,7 +1280,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1308,7 +1308,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1318,7 +1318,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1330,13 +1330,13 @@
         <v>1</v>
       </c>
       <c r="F32" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1364,7 +1364,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1392,7 +1392,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1402,7 +1402,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1414,13 +1414,13 @@
         <v>1</v>
       </c>
       <c r="F35" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1430,7 +1430,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1442,13 +1442,13 @@
         <v>1</v>
       </c>
       <c r="F36" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1458,7 +1458,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1470,13 +1470,13 @@
         <v>1</v>
       </c>
       <c r="F37" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1486,7 +1486,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1498,13 +1498,13 @@
         <v>1</v>
       </c>
       <c r="F38" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1532,7 +1532,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1560,7 +1560,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1588,7 +1588,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1616,7 +1616,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1644,7 +1644,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1672,7 +1672,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1694,13 +1694,13 @@
         <v>1</v>
       </c>
       <c r="F45" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1710,7 +1710,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1722,13 +1722,13 @@
         <v>1</v>
       </c>
       <c r="F46" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1738,7 +1738,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1750,13 +1750,13 @@
         <v>1</v>
       </c>
       <c r="F47" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1766,7 +1766,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1778,13 +1778,13 @@
         <v>1</v>
       </c>
       <c r="F48" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1812,7 +1812,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1840,7 +1840,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -1862,13 +1862,13 @@
         <v>1</v>
       </c>
       <c r="F51" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1896,7 +1896,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1924,7 +1924,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1952,7 +1952,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1980,7 +1980,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -2008,7 +2008,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -2036,7 +2036,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -2064,7 +2064,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -2092,7 +2092,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -2120,7 +2120,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -2148,7 +2148,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -2176,7 +2176,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -2204,7 +2204,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -2232,7 +2232,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -2254,13 +2254,13 @@
         <v>1</v>
       </c>
       <c r="F65" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2316,7 +2316,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -2344,7 +2344,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -2372,7 +2372,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -2400,7 +2400,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2410,7 +2410,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -2422,13 +2422,13 @@
         <v>1</v>
       </c>
       <c r="F71" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2438,7 +2438,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -2450,13 +2450,13 @@
         <v>1</v>
       </c>
       <c r="F72" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2484,7 +2484,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -2512,7 +2512,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2540,7 +2540,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2568,7 +2568,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2596,7 +2596,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2606,7 +2606,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -2618,13 +2618,13 @@
         <v>1</v>
       </c>
       <c r="F78" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2652,7 +2652,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2680,7 +2680,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -2736,7 +2736,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -2764,7 +2764,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -2792,7 +2792,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2802,7 +2802,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -2814,13 +2814,13 @@
         <v>1</v>
       </c>
       <c r="F85" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2848,7 +2848,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -2876,7 +2876,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2886,7 +2886,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -2898,13 +2898,13 @@
         <v>1</v>
       </c>
       <c r="F88" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2914,7 +2914,7 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -2926,13 +2926,13 @@
         <v>1</v>
       </c>
       <c r="F89" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -2960,7 +2960,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -2988,7 +2988,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -2998,7 +2998,7 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -3010,13 +3010,13 @@
         <v>1</v>
       </c>
       <c r="F92" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -3026,7 +3026,7 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -3038,13 +3038,13 @@
         <v>1</v>
       </c>
       <c r="F93" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -3072,7 +3072,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -3100,7 +3100,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -3156,7 +3156,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -3166,7 +3166,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -3178,13 +3178,13 @@
         <v>1</v>
       </c>
       <c r="F98" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -3212,7 +3212,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -3222,7 +3222,7 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -3234,13 +3234,13 @@
         <v>1</v>
       </c>
       <c r="F100" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -3268,7 +3268,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -3296,7 +3296,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -3324,7 +3324,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -3352,7 +3352,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -3380,7 +3380,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -3408,7 +3408,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -3436,7 +3436,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -3464,7 +3464,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -3492,7 +3492,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -3502,7 +3502,7 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -3514,13 +3514,13 @@
         <v>1</v>
       </c>
       <c r="F110" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -3530,7 +3530,7 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -3542,13 +3542,13 @@
         <v>1</v>
       </c>
       <c r="F111" t="n">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3558,7 +3558,7 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -3570,13 +3570,13 @@
         <v>1</v>
       </c>
       <c r="F112" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3586,7 +3586,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -3598,13 +3598,13 @@
         <v>1</v>
       </c>
       <c r="F113" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -3614,7 +3614,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -3626,13 +3626,13 @@
         <v>1</v>
       </c>
       <c r="F114" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -3660,7 +3660,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
@@ -3688,7 +3688,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -3716,7 +3716,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -3726,7 +3726,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
@@ -3738,13 +3738,13 @@
         <v>1</v>
       </c>
       <c r="F118" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -3754,7 +3754,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
@@ -3766,13 +3766,13 @@
         <v>1</v>
       </c>
       <c r="F119" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -3800,7 +3800,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -3828,7 +3828,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -3856,7 +3856,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -3884,7 +3884,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -3912,7 +3912,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -3940,7 +3940,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -3968,7 +3968,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -3978,7 +3978,7 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
@@ -3990,13 +3990,13 @@
         <v>1</v>
       </c>
       <c r="F127" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -4024,7 +4024,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -4034,7 +4034,7 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
@@ -4046,13 +4046,13 @@
         <v>1</v>
       </c>
       <c r="F129" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -4080,7 +4080,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -4108,7 +4108,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -4136,7 +4136,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -4164,7 +4164,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -4192,7 +4192,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -4220,7 +4220,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -4248,7 +4248,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -4276,7 +4276,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -4286,7 +4286,7 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
@@ -4298,13 +4298,13 @@
         <v>1</v>
       </c>
       <c r="F138" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
@@ -4332,7 +4332,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -4342,7 +4342,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
@@ -4354,13 +4354,13 @@
         <v>1</v>
       </c>
       <c r="F140" t="n">
-        <v>60</v>
+        <v>35</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -4370,7 +4370,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
@@ -4382,13 +4382,13 @@
         <v>1</v>
       </c>
       <c r="F141" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -4416,7 +4416,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -4444,7 +4444,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -4472,7 +4472,7 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
@@ -4482,7 +4482,7 @@
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
@@ -4494,13 +4494,13 @@
         <v>1</v>
       </c>
       <c r="F145" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
@@ -4510,7 +4510,7 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
@@ -4522,13 +4522,13 @@
         <v>1</v>
       </c>
       <c r="F146" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -4556,7 +4556,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -4566,7 +4566,7 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
@@ -4578,13 +4578,13 @@
         <v>1</v>
       </c>
       <c r="F148" t="n">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
@@ -4612,7 +4612,7 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
@@ -4640,7 +4640,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -4668,7 +4668,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -4678,7 +4678,7 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
@@ -4690,13 +4690,13 @@
         <v>1</v>
       </c>
       <c r="F152" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -4706,7 +4706,7 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
@@ -4718,13 +4718,13 @@
         <v>1</v>
       </c>
       <c r="F153" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -4734,7 +4734,7 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D154" t="inlineStr">
@@ -4746,13 +4746,13 @@
         <v>1</v>
       </c>
       <c r="F154" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
@@ -4780,7 +4780,7 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
@@ -4808,7 +4808,7 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
@@ -4836,7 +4836,7 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
@@ -4846,7 +4846,7 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
@@ -4858,13 +4858,13 @@
         <v>1</v>
       </c>
       <c r="F158" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
@@ -4892,7 +4892,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -4920,7 +4920,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -4942,13 +4942,13 @@
         <v>1</v>
       </c>
       <c r="F161" t="n">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -4976,7 +4976,7 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
@@ -5004,7 +5004,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
@@ -5014,7 +5014,7 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
       <c r="D164" t="inlineStr">
@@ -5026,13 +5026,13 @@
         <v>1</v>
       </c>
       <c r="F164" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -5060,7 +5060,7 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
@@ -5088,7 +5088,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
@@ -5116,7 +5116,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
@@ -5144,7 +5144,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
@@ -5172,7 +5172,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
@@ -5200,7 +5200,7 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
@@ -5228,7 +5228,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
@@ -5256,7 +5256,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
@@ -5284,7 +5284,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -5312,7 +5312,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -5340,7 +5340,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -5350,7 +5350,7 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D176" t="inlineStr">
@@ -5362,13 +5362,13 @@
         <v>1</v>
       </c>
       <c r="F176" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -5396,7 +5396,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -5406,7 +5406,7 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D178" t="inlineStr">
@@ -5418,13 +5418,13 @@
         <v>1</v>
       </c>
       <c r="F178" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
@@ -5452,7 +5452,7 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
@@ -5480,7 +5480,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
@@ -5490,7 +5490,7 @@
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D181" t="inlineStr">
@@ -5502,13 +5502,13 @@
         <v>1</v>
       </c>
       <c r="F181" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
@@ -5536,7 +5536,7 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
@@ -5564,7 +5564,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
@@ -5574,7 +5574,7 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
       <c r="D184" t="inlineStr">
@@ -5586,13 +5586,13 @@
         <v>1</v>
       </c>
       <c r="F184" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
@@ -5602,7 +5602,7 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D185" t="inlineStr">
@@ -5614,13 +5614,13 @@
         <v>1</v>
       </c>
       <c r="F185" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -5642,13 +5642,13 @@
         <v>1</v>
       </c>
       <c r="F186" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5676,7 +5676,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5704,7 +5704,7 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
@@ -5714,7 +5714,7 @@
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D189" t="inlineStr">
@@ -5726,13 +5726,13 @@
         <v>1</v>
       </c>
       <c r="F189" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
@@ -5760,7 +5760,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
@@ -5788,7 +5788,7 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
@@ -5816,7 +5816,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
@@ -5844,7 +5844,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -5872,7 +5872,7 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
@@ -5900,7 +5900,7 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
@@ -5928,7 +5928,7 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
@@ -5956,7 +5956,7 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
@@ -5966,7 +5966,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D198" t="inlineStr">
@@ -5978,13 +5978,13 @@
         <v>1</v>
       </c>
       <c r="F198" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
@@ -6012,7 +6012,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
@@ -6022,7 +6022,7 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D200" t="inlineStr">
@@ -6034,13 +6034,13 @@
         <v>1</v>
       </c>
       <c r="F200" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
@@ -6050,7 +6050,7 @@
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D201" t="inlineStr">
@@ -6062,13 +6062,13 @@
         <v>1</v>
       </c>
       <c r="F201" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
@@ -6096,7 +6096,7 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
@@ -6124,7 +6124,7 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
@@ -6152,7 +6152,7 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
@@ -6180,7 +6180,7 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
@@ -6208,7 +6208,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
@@ -6236,7 +6236,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -6264,7 +6264,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
@@ -6274,7 +6274,7 @@
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D209" t="inlineStr">
@@ -6286,13 +6286,13 @@
         <v>1</v>
       </c>
       <c r="F209" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
@@ -6320,7 +6320,7 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
@@ -6348,7 +6348,7 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
@@ -6358,7 +6358,7 @@
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D212" t="inlineStr">
@@ -6370,13 +6370,13 @@
         <v>1</v>
       </c>
       <c r="F212" t="n">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
@@ -6386,7 +6386,7 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D213" t="inlineStr">
@@ -6398,13 +6398,13 @@
         <v>1</v>
       </c>
       <c r="F213" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
@@ -6432,7 +6432,7 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
@@ -6460,7 +6460,7 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
@@ -6488,7 +6488,7 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
@@ -6516,7 +6516,7 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
@@ -6544,7 +6544,7 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
@@ -6554,7 +6554,7 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D219" t="inlineStr">
@@ -6566,13 +6566,13 @@
         <v>1</v>
       </c>
       <c r="F219" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
@@ -6600,7 +6600,7 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
@@ -6622,13 +6622,13 @@
         <v>1</v>
       </c>
       <c r="F221" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
@@ -6656,7 +6656,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
@@ -6684,7 +6684,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
@@ -6712,7 +6712,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
@@ -6740,7 +6740,7 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
@@ -6750,7 +6750,7 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D226" t="inlineStr">
@@ -6762,13 +6762,13 @@
         <v>1</v>
       </c>
       <c r="F226" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
@@ -6796,7 +6796,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
@@ -6806,7 +6806,7 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D228" t="inlineStr">
@@ -6818,13 +6818,13 @@
         <v>1</v>
       </c>
       <c r="F228" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -6852,7 +6852,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -6862,7 +6862,7 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D230" t="inlineStr">
@@ -6874,13 +6874,13 @@
         <v>1</v>
       </c>
       <c r="F230" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
@@ -6890,7 +6890,7 @@
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D231" t="inlineStr">
@@ -6902,13 +6902,13 @@
         <v>1</v>
       </c>
       <c r="F231" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
@@ -6918,7 +6918,7 @@
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D232" t="inlineStr">
@@ -6930,13 +6930,13 @@
         <v>1</v>
       </c>
       <c r="F232" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
@@ -6964,7 +6964,7 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
@@ -6974,7 +6974,7 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D234" t="inlineStr">
@@ -6986,13 +6986,13 @@
         <v>1</v>
       </c>
       <c r="F234" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
@@ -7020,7 +7020,7 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
@@ -7042,13 +7042,13 @@
         <v>1</v>
       </c>
       <c r="F236" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
@@ -7058,7 +7058,7 @@
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D237" t="inlineStr">
@@ -7070,13 +7070,13 @@
         <v>1</v>
       </c>
       <c r="F237" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
@@ -7104,7 +7104,7 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
@@ -7132,7 +7132,7 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
@@ -7160,7 +7160,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -7188,7 +7188,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
@@ -7198,7 +7198,7 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D242" t="inlineStr">
@@ -7210,13 +7210,13 @@
         <v>1</v>
       </c>
       <c r="F242" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
@@ -7244,7 +7244,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
@@ -7272,7 +7272,7 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
@@ -7300,7 +7300,7 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
@@ -7310,7 +7310,7 @@
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D246" t="inlineStr">
@@ -7322,13 +7322,13 @@
         <v>1</v>
       </c>
       <c r="F246" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
@@ -7338,7 +7338,7 @@
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D247" t="inlineStr">
@@ -7350,13 +7350,13 @@
         <v>1</v>
       </c>
       <c r="F247" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
@@ -7384,7 +7384,7 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
@@ -7412,7 +7412,7 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
@@ -7440,7 +7440,7 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
@@ -7468,7 +7468,7 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
@@ -7496,7 +7496,7 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
@@ -7524,7 +7524,7 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
@@ -7552,7 +7552,7 @@
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
@@ -7580,7 +7580,7 @@
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
@@ -7608,7 +7608,7 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
@@ -7618,7 +7618,7 @@
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D257" t="inlineStr">
@@ -7630,13 +7630,13 @@
         <v>1</v>
       </c>
       <c r="F257" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
@@ -7646,7 +7646,7 @@
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="D258" t="inlineStr">
@@ -7658,13 +7658,13 @@
         <v>1</v>
       </c>
       <c r="F258" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
@@ -7692,7 +7692,7 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>2025-07-24 03:04:11</t>
+          <t>2025-07-24 03:52:11</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">

</xml_diff>

<commit_message>
Atualização automática [Thu Jul 24 04:04:37 UTC 2025]
</commit_message>
<xml_diff>
--- a/livelo_parceiros.xlsx
+++ b/livelo_parceiros.xlsx
@@ -468,7 +468,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -496,7 +496,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -524,7 +524,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -552,7 +552,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -580,7 +580,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -636,7 +636,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -664,7 +664,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -692,7 +692,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -720,7 +720,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -748,7 +748,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -776,7 +776,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -804,7 +804,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -832,7 +832,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -860,7 +860,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -888,7 +888,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -916,7 +916,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -944,7 +944,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -972,7 +972,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1000,7 +1000,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1056,7 +1056,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1084,7 +1084,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1112,7 +1112,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1140,7 +1140,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1168,7 +1168,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1196,7 +1196,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1224,7 +1224,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1252,7 +1252,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1280,7 +1280,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1308,7 +1308,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1336,7 +1336,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1364,7 +1364,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1392,7 +1392,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1420,7 +1420,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1476,7 +1476,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1504,7 +1504,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1532,7 +1532,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1560,7 +1560,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1588,7 +1588,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1616,7 +1616,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1644,7 +1644,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1672,7 +1672,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1700,7 +1700,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1728,7 +1728,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1756,7 +1756,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1784,7 +1784,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1812,7 +1812,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1840,7 +1840,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1896,7 +1896,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1924,7 +1924,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1952,7 +1952,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1980,7 +1980,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -2008,7 +2008,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -2036,7 +2036,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -2064,7 +2064,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -2092,7 +2092,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -2120,7 +2120,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -2148,7 +2148,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -2176,7 +2176,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -2204,7 +2204,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -2232,7 +2232,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -2260,7 +2260,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2316,7 +2316,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -2344,7 +2344,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -2372,7 +2372,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -2400,7 +2400,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2428,7 +2428,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2456,7 +2456,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2484,7 +2484,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -2512,7 +2512,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2540,7 +2540,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2568,7 +2568,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2596,7 +2596,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2624,7 +2624,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2652,7 +2652,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2680,7 +2680,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -2736,7 +2736,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -2764,7 +2764,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -2792,7 +2792,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2820,7 +2820,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2848,7 +2848,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -2876,7 +2876,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2904,7 +2904,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2932,7 +2932,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -2960,7 +2960,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -2988,7 +2988,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -3016,7 +3016,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -3044,7 +3044,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -3072,7 +3072,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -3100,7 +3100,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -3156,7 +3156,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -3184,7 +3184,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -3212,7 +3212,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -3240,7 +3240,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -3268,7 +3268,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -3296,7 +3296,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -3324,7 +3324,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -3352,7 +3352,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -3380,7 +3380,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -3408,7 +3408,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -3436,7 +3436,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -3464,7 +3464,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -3492,7 +3492,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -3520,7 +3520,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -3548,7 +3548,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3576,7 +3576,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3604,7 +3604,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -3632,7 +3632,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -3660,7 +3660,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
@@ -3688,7 +3688,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -3716,7 +3716,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -3744,7 +3744,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -3772,7 +3772,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -3800,7 +3800,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -3828,7 +3828,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -3856,7 +3856,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -3884,7 +3884,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -3912,7 +3912,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -3940,7 +3940,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -3968,7 +3968,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -3996,7 +3996,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -4024,7 +4024,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -4052,7 +4052,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -4080,7 +4080,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -4108,7 +4108,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -4136,7 +4136,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -4164,7 +4164,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -4192,7 +4192,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -4220,7 +4220,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -4248,7 +4248,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -4276,7 +4276,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -4304,7 +4304,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
@@ -4332,7 +4332,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -4360,7 +4360,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -4388,7 +4388,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -4416,7 +4416,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -4444,7 +4444,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -4472,7 +4472,7 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
@@ -4500,7 +4500,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
@@ -4528,7 +4528,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -4556,7 +4556,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -4584,7 +4584,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
@@ -4612,7 +4612,7 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
@@ -4640,7 +4640,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -4668,7 +4668,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -4696,7 +4696,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -4724,7 +4724,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -4752,7 +4752,7 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
@@ -4780,7 +4780,7 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
@@ -4808,7 +4808,7 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
@@ -4836,7 +4836,7 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
@@ -4864,7 +4864,7 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
@@ -4892,7 +4892,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -4920,7 +4920,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -4948,7 +4948,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -4976,7 +4976,7 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
@@ -5004,7 +5004,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
@@ -5032,7 +5032,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -5060,7 +5060,7 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
@@ -5088,7 +5088,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
@@ -5116,7 +5116,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
@@ -5144,7 +5144,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
@@ -5172,7 +5172,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
@@ -5200,7 +5200,7 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
@@ -5228,7 +5228,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
@@ -5256,7 +5256,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
@@ -5284,7 +5284,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -5312,7 +5312,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -5340,7 +5340,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -5368,7 +5368,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -5396,7 +5396,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -5424,7 +5424,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
@@ -5452,7 +5452,7 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
@@ -5480,7 +5480,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
@@ -5508,7 +5508,7 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
@@ -5536,7 +5536,7 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
@@ -5564,7 +5564,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
@@ -5592,7 +5592,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
@@ -5620,7 +5620,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -5648,7 +5648,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5676,7 +5676,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5704,7 +5704,7 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
@@ -5732,7 +5732,7 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
@@ -5760,7 +5760,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
@@ -5788,7 +5788,7 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
@@ -5816,7 +5816,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
@@ -5844,7 +5844,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -5872,7 +5872,7 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
@@ -5900,7 +5900,7 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
@@ -5928,7 +5928,7 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
@@ -5956,7 +5956,7 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
@@ -5984,7 +5984,7 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
@@ -6012,7 +6012,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
@@ -6040,7 +6040,7 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
@@ -6068,7 +6068,7 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
@@ -6096,7 +6096,7 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
@@ -6124,7 +6124,7 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
@@ -6152,7 +6152,7 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
@@ -6180,7 +6180,7 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
@@ -6208,7 +6208,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
@@ -6236,7 +6236,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -6264,7 +6264,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
@@ -6292,7 +6292,7 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
@@ -6320,7 +6320,7 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
@@ -6348,7 +6348,7 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
@@ -6376,7 +6376,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
@@ -6404,7 +6404,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
@@ -6432,7 +6432,7 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
@@ -6460,7 +6460,7 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
@@ -6488,7 +6488,7 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
@@ -6516,7 +6516,7 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
@@ -6544,7 +6544,7 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
@@ -6572,7 +6572,7 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
@@ -6600,7 +6600,7 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
@@ -6628,7 +6628,7 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
@@ -6656,7 +6656,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
@@ -6684,7 +6684,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
@@ -6712,7 +6712,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
@@ -6740,7 +6740,7 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
@@ -6768,7 +6768,7 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
@@ -6796,7 +6796,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
@@ -6824,7 +6824,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -6852,7 +6852,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -6880,7 +6880,7 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
@@ -6908,7 +6908,7 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
@@ -6936,7 +6936,7 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
@@ -6964,7 +6964,7 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
@@ -6992,7 +6992,7 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
@@ -7020,7 +7020,7 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
@@ -7048,7 +7048,7 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
@@ -7076,7 +7076,7 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
@@ -7104,7 +7104,7 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
@@ -7132,7 +7132,7 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
@@ -7160,7 +7160,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -7188,7 +7188,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
@@ -7216,7 +7216,7 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
@@ -7244,7 +7244,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
@@ -7272,7 +7272,7 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
@@ -7300,7 +7300,7 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
@@ -7328,7 +7328,7 @@
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
@@ -7356,7 +7356,7 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
@@ -7384,7 +7384,7 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
@@ -7412,7 +7412,7 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
@@ -7440,7 +7440,7 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
@@ -7468,7 +7468,7 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
@@ -7496,7 +7496,7 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
@@ -7524,7 +7524,7 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
@@ -7552,7 +7552,7 @@
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
@@ -7580,7 +7580,7 @@
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
@@ -7608,7 +7608,7 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
@@ -7636,7 +7636,7 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
@@ -7664,7 +7664,7 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
@@ -7692,7 +7692,7 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>2025-07-24 03:52:11</t>
+          <t>2025-07-24 04:04:16</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">

</xml_diff>

<commit_message>
Atualização automática [Thu Jul 24 12:22:29 UTC 2025]
</commit_message>
<xml_diff>
--- a/livelo_parceiros.xlsx
+++ b/livelo_parceiros.xlsx
@@ -468,7 +468,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -496,7 +496,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -524,7 +524,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -552,7 +552,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -580,7 +580,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -636,7 +636,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -664,7 +664,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -692,7 +692,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -720,7 +720,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -748,7 +748,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -776,7 +776,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -804,7 +804,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -832,7 +832,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -860,7 +860,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -888,7 +888,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -916,7 +916,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -944,7 +944,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -972,7 +972,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1000,7 +1000,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1056,7 +1056,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1084,7 +1084,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1112,7 +1112,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1140,7 +1140,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1168,7 +1168,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1196,7 +1196,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1224,7 +1224,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1252,7 +1252,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1280,7 +1280,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1308,7 +1308,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1336,7 +1336,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1364,7 +1364,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1392,7 +1392,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1420,7 +1420,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1476,7 +1476,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1504,7 +1504,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1532,7 +1532,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1560,7 +1560,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1588,7 +1588,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1616,7 +1616,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1644,7 +1644,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1672,7 +1672,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1700,7 +1700,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1728,7 +1728,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1756,7 +1756,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1784,7 +1784,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1812,7 +1812,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1840,7 +1840,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1896,7 +1896,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1924,7 +1924,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1952,7 +1952,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1980,7 +1980,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -2008,7 +2008,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -2036,7 +2036,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -2064,7 +2064,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -2092,7 +2092,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -2120,7 +2120,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -2148,7 +2148,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -2176,7 +2176,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -2204,7 +2204,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -2232,7 +2232,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -2260,7 +2260,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2316,7 +2316,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -2344,7 +2344,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -2372,7 +2372,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -2400,7 +2400,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2428,7 +2428,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2456,7 +2456,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2484,7 +2484,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -2512,7 +2512,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2540,7 +2540,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2568,7 +2568,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2596,7 +2596,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2624,7 +2624,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2652,7 +2652,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2680,7 +2680,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -2736,7 +2736,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -2764,7 +2764,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -2792,7 +2792,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2820,7 +2820,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2848,7 +2848,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -2876,7 +2876,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2904,7 +2904,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2932,7 +2932,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -2960,7 +2960,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -2988,7 +2988,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -3016,7 +3016,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -3044,7 +3044,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -3072,7 +3072,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -3100,7 +3100,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -3156,7 +3156,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -3184,7 +3184,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -3212,7 +3212,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -3240,7 +3240,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -3268,7 +3268,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -3296,7 +3296,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -3324,7 +3324,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -3352,7 +3352,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -3380,7 +3380,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -3408,7 +3408,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -3436,7 +3436,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -3464,7 +3464,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -3492,7 +3492,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -3520,7 +3520,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -3548,7 +3548,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3576,7 +3576,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3604,7 +3604,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -3632,7 +3632,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -3660,7 +3660,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
@@ -3688,7 +3688,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -3716,7 +3716,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -3744,7 +3744,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -3772,7 +3772,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -3800,7 +3800,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -3828,7 +3828,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -3856,7 +3856,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -3884,7 +3884,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -3912,7 +3912,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -3940,7 +3940,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -3968,7 +3968,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -3996,7 +3996,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -4024,7 +4024,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -4052,7 +4052,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -4080,7 +4080,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -4108,7 +4108,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -4136,7 +4136,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -4164,7 +4164,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -4192,7 +4192,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -4220,7 +4220,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -4248,7 +4248,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -4276,7 +4276,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -4304,7 +4304,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
@@ -4332,7 +4332,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -4360,7 +4360,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -4388,7 +4388,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -4416,7 +4416,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -4444,7 +4444,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -4472,7 +4472,7 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
@@ -4500,7 +4500,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
@@ -4528,7 +4528,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -4556,7 +4556,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -4584,7 +4584,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
@@ -4612,7 +4612,7 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
@@ -4640,7 +4640,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -4668,7 +4668,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -4696,7 +4696,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -4724,7 +4724,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -4752,7 +4752,7 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
@@ -4780,7 +4780,7 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
@@ -4808,7 +4808,7 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
@@ -4836,7 +4836,7 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
@@ -4864,7 +4864,7 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
@@ -4892,7 +4892,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -4920,7 +4920,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -4948,7 +4948,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -4976,7 +4976,7 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
@@ -5004,7 +5004,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
@@ -5032,7 +5032,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -5060,7 +5060,7 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
@@ -5088,7 +5088,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
@@ -5116,7 +5116,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
@@ -5144,7 +5144,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
@@ -5172,7 +5172,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
@@ -5200,7 +5200,7 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
@@ -5228,7 +5228,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
@@ -5256,7 +5256,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
@@ -5284,7 +5284,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -5312,7 +5312,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -5340,7 +5340,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -5368,7 +5368,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -5396,7 +5396,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -5424,7 +5424,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
@@ -5452,7 +5452,7 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
@@ -5480,7 +5480,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
@@ -5508,7 +5508,7 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
@@ -5536,7 +5536,7 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
@@ -5564,7 +5564,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
@@ -5592,7 +5592,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
@@ -5620,7 +5620,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -5648,7 +5648,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5676,7 +5676,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5704,7 +5704,7 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
@@ -5732,7 +5732,7 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
@@ -5760,7 +5760,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
@@ -5788,7 +5788,7 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
@@ -5816,7 +5816,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
@@ -5844,7 +5844,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -5872,7 +5872,7 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
@@ -5900,7 +5900,7 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
@@ -5928,7 +5928,7 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
@@ -5956,7 +5956,7 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
@@ -5984,7 +5984,7 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
@@ -6012,7 +6012,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
@@ -6040,7 +6040,7 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
@@ -6068,7 +6068,7 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
@@ -6096,7 +6096,7 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
@@ -6124,7 +6124,7 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
@@ -6152,7 +6152,7 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
@@ -6180,7 +6180,7 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
@@ -6208,7 +6208,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
@@ -6236,7 +6236,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -6264,7 +6264,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
@@ -6292,7 +6292,7 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
@@ -6320,7 +6320,7 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
@@ -6348,7 +6348,7 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
@@ -6376,7 +6376,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
@@ -6404,7 +6404,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
@@ -6432,7 +6432,7 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
@@ -6460,7 +6460,7 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
@@ -6488,7 +6488,7 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
@@ -6516,7 +6516,7 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
@@ -6544,7 +6544,7 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
@@ -6572,7 +6572,7 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
@@ -6600,7 +6600,7 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
@@ -6628,7 +6628,7 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
@@ -6656,7 +6656,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
@@ -6684,7 +6684,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
@@ -6712,7 +6712,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
@@ -6740,7 +6740,7 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
@@ -6768,7 +6768,7 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
@@ -6796,7 +6796,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
@@ -6824,7 +6824,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -6852,7 +6852,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -6880,7 +6880,7 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
@@ -6908,7 +6908,7 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
@@ -6936,7 +6936,7 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
@@ -6964,7 +6964,7 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
@@ -6992,7 +6992,7 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
@@ -7020,7 +7020,7 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
@@ -7048,7 +7048,7 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
@@ -7076,7 +7076,7 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
@@ -7104,7 +7104,7 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
@@ -7132,7 +7132,7 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
@@ -7160,7 +7160,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -7188,7 +7188,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
@@ -7216,7 +7216,7 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
@@ -7244,7 +7244,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
@@ -7272,7 +7272,7 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
@@ -7300,7 +7300,7 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
@@ -7328,7 +7328,7 @@
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
@@ -7356,7 +7356,7 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
@@ -7384,7 +7384,7 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
@@ -7412,7 +7412,7 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
@@ -7440,7 +7440,7 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
@@ -7468,7 +7468,7 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
@@ -7496,7 +7496,7 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
@@ -7524,7 +7524,7 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
@@ -7552,7 +7552,7 @@
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
@@ -7580,7 +7580,7 @@
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
@@ -7608,7 +7608,7 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
@@ -7636,7 +7636,7 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
@@ -7664,7 +7664,7 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
@@ -7692,7 +7692,7 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>2025-07-24 04:04:16</t>
+          <t>2025-07-24 12:22:08</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">

</xml_diff>

<commit_message>
Atualização automática [Fri Jul 25 13:49:11 UTC 2025]
</commit_message>
<xml_diff>
--- a/livelo_parceiros.xlsx
+++ b/livelo_parceiros.xlsx
@@ -7720,7 +7720,7 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
@@ -7748,7 +7748,7 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
@@ -7776,7 +7776,7 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
@@ -7804,7 +7804,7 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
@@ -7832,7 +7832,7 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
@@ -7860,7 +7860,7 @@
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
@@ -7888,7 +7888,7 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
@@ -7916,7 +7916,7 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
@@ -7944,7 +7944,7 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
@@ -7972,7 +7972,7 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
@@ -8000,7 +8000,7 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
@@ -8028,7 +8028,7 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
@@ -8056,7 +8056,7 @@
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
@@ -8084,7 +8084,7 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
@@ -8112,7 +8112,7 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
@@ -8140,7 +8140,7 @@
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
@@ -8168,7 +8168,7 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
@@ -8196,7 +8196,7 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
@@ -8224,7 +8224,7 @@
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
@@ -8252,7 +8252,7 @@
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
@@ -8280,7 +8280,7 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
@@ -8308,7 +8308,7 @@
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
@@ -8336,7 +8336,7 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
@@ -8364,7 +8364,7 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
@@ -8392,7 +8392,7 @@
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
@@ -8420,7 +8420,7 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
@@ -8448,7 +8448,7 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
@@ -8476,7 +8476,7 @@
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
@@ -8504,7 +8504,7 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
@@ -8532,7 +8532,7 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
@@ -8560,7 +8560,7 @@
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
@@ -8588,7 +8588,7 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
@@ -8616,7 +8616,7 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
@@ -8644,7 +8644,7 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
@@ -8672,7 +8672,7 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
@@ -8700,7 +8700,7 @@
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
@@ -8728,7 +8728,7 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
@@ -8756,7 +8756,7 @@
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
@@ -8784,7 +8784,7 @@
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
@@ -8812,7 +8812,7 @@
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
@@ -8822,7 +8822,7 @@
       </c>
       <c r="C300" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
       <c r="D300" t="inlineStr">
@@ -8834,13 +8834,13 @@
         <v>1</v>
       </c>
       <c r="F300" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
@@ -8868,7 +8868,7 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
@@ -8896,7 +8896,7 @@
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
@@ -8924,7 +8924,7 @@
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
@@ -8952,7 +8952,7 @@
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
@@ -8980,7 +8980,7 @@
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
@@ -9008,7 +9008,7 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
@@ -9036,7 +9036,7 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
@@ -9064,7 +9064,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
@@ -9092,7 +9092,7 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
@@ -9120,7 +9120,7 @@
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
@@ -9148,7 +9148,7 @@
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
@@ -9176,7 +9176,7 @@
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
@@ -9204,7 +9204,7 @@
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
@@ -9232,7 +9232,7 @@
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
@@ -9260,7 +9260,7 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
@@ -9288,7 +9288,7 @@
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
@@ -9316,7 +9316,7 @@
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
@@ -9344,7 +9344,7 @@
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
@@ -9372,7 +9372,7 @@
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
@@ -9400,7 +9400,7 @@
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
@@ -9428,7 +9428,7 @@
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
@@ -9456,7 +9456,7 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
@@ -9484,7 +9484,7 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
@@ -9512,7 +9512,7 @@
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
@@ -9540,7 +9540,7 @@
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
@@ -9568,7 +9568,7 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
@@ -9596,7 +9596,7 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
@@ -9624,7 +9624,7 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
@@ -9652,7 +9652,7 @@
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
@@ -9680,7 +9680,7 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
@@ -9708,7 +9708,7 @@
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
@@ -9736,7 +9736,7 @@
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B333" t="inlineStr">
@@ -9764,7 +9764,7 @@
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B334" t="inlineStr">
@@ -9792,7 +9792,7 @@
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B335" t="inlineStr">
@@ -9820,7 +9820,7 @@
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B336" t="inlineStr">
@@ -9848,7 +9848,7 @@
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B337" t="inlineStr">
@@ -9876,7 +9876,7 @@
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B338" t="inlineStr">
@@ -9904,7 +9904,7 @@
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B339" t="inlineStr">
@@ -9932,7 +9932,7 @@
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B340" t="inlineStr">
@@ -9960,7 +9960,7 @@
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B341" t="inlineStr">
@@ -9988,7 +9988,7 @@
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B342" t="inlineStr">
@@ -10016,7 +10016,7 @@
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B343" t="inlineStr">
@@ -10044,7 +10044,7 @@
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B344" t="inlineStr">
@@ -10072,7 +10072,7 @@
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B345" t="inlineStr">
@@ -10100,7 +10100,7 @@
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B346" t="inlineStr">
@@ -10128,7 +10128,7 @@
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B347" t="inlineStr">
@@ -10156,7 +10156,7 @@
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B348" t="inlineStr">
@@ -10184,7 +10184,7 @@
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B349" t="inlineStr">
@@ -10212,7 +10212,7 @@
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B350" t="inlineStr">
@@ -10240,7 +10240,7 @@
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B351" t="inlineStr">
@@ -10268,7 +10268,7 @@
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B352" t="inlineStr">
@@ -10296,7 +10296,7 @@
     <row r="353">
       <c r="A353" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B353" t="inlineStr">
@@ -10324,7 +10324,7 @@
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B354" t="inlineStr">
@@ -10352,7 +10352,7 @@
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B355" t="inlineStr">
@@ -10380,7 +10380,7 @@
     <row r="356">
       <c r="A356" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B356" t="inlineStr">
@@ -10408,7 +10408,7 @@
     <row r="357">
       <c r="A357" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B357" t="inlineStr">
@@ -10436,7 +10436,7 @@
     <row r="358">
       <c r="A358" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B358" t="inlineStr">
@@ -10464,7 +10464,7 @@
     <row r="359">
       <c r="A359" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B359" t="inlineStr">
@@ -10492,7 +10492,7 @@
     <row r="360">
       <c r="A360" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B360" t="inlineStr">
@@ -10520,7 +10520,7 @@
     <row r="361">
       <c r="A361" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B361" t="inlineStr">
@@ -10548,7 +10548,7 @@
     <row r="362">
       <c r="A362" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B362" t="inlineStr">
@@ -10576,7 +10576,7 @@
     <row r="363">
       <c r="A363" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B363" t="inlineStr">
@@ -10604,7 +10604,7 @@
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B364" t="inlineStr">
@@ -10632,7 +10632,7 @@
     <row r="365">
       <c r="A365" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B365" t="inlineStr">
@@ -10660,7 +10660,7 @@
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B366" t="inlineStr">
@@ -10688,7 +10688,7 @@
     <row r="367">
       <c r="A367" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B367" t="inlineStr">
@@ -10716,7 +10716,7 @@
     <row r="368">
       <c r="A368" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B368" t="inlineStr">
@@ -10744,7 +10744,7 @@
     <row r="369">
       <c r="A369" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B369" t="inlineStr">
@@ -10772,7 +10772,7 @@
     <row r="370">
       <c r="A370" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B370" t="inlineStr">
@@ -10800,7 +10800,7 @@
     <row r="371">
       <c r="A371" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B371" t="inlineStr">
@@ -10828,7 +10828,7 @@
     <row r="372">
       <c r="A372" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B372" t="inlineStr">
@@ -10856,7 +10856,7 @@
     <row r="373">
       <c r="A373" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B373" t="inlineStr">
@@ -10884,7 +10884,7 @@
     <row r="374">
       <c r="A374" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B374" t="inlineStr">
@@ -10912,7 +10912,7 @@
     <row r="375">
       <c r="A375" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B375" t="inlineStr">
@@ -10940,7 +10940,7 @@
     <row r="376">
       <c r="A376" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B376" t="inlineStr">
@@ -10968,7 +10968,7 @@
     <row r="377">
       <c r="A377" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B377" t="inlineStr">
@@ -10996,7 +10996,7 @@
     <row r="378">
       <c r="A378" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B378" t="inlineStr">
@@ -11024,7 +11024,7 @@
     <row r="379">
       <c r="A379" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B379" t="inlineStr">
@@ -11052,7 +11052,7 @@
     <row r="380">
       <c r="A380" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B380" t="inlineStr">
@@ -11080,7 +11080,7 @@
     <row r="381">
       <c r="A381" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B381" t="inlineStr">
@@ -11108,7 +11108,7 @@
     <row r="382">
       <c r="A382" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B382" t="inlineStr">
@@ -11136,7 +11136,7 @@
     <row r="383">
       <c r="A383" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B383" t="inlineStr">
@@ -11164,7 +11164,7 @@
     <row r="384">
       <c r="A384" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B384" t="inlineStr">
@@ -11192,7 +11192,7 @@
     <row r="385">
       <c r="A385" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B385" t="inlineStr">
@@ -11220,7 +11220,7 @@
     <row r="386">
       <c r="A386" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B386" t="inlineStr">
@@ -11248,7 +11248,7 @@
     <row r="387">
       <c r="A387" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B387" t="inlineStr">
@@ -11276,7 +11276,7 @@
     <row r="388">
       <c r="A388" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B388" t="inlineStr">
@@ -11304,7 +11304,7 @@
     <row r="389">
       <c r="A389" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B389" t="inlineStr">
@@ -11332,7 +11332,7 @@
     <row r="390">
       <c r="A390" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B390" t="inlineStr">
@@ -11360,7 +11360,7 @@
     <row r="391">
       <c r="A391" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B391" t="inlineStr">
@@ -11388,7 +11388,7 @@
     <row r="392">
       <c r="A392" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B392" t="inlineStr">
@@ -11416,7 +11416,7 @@
     <row r="393">
       <c r="A393" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B393" t="inlineStr">
@@ -11444,7 +11444,7 @@
     <row r="394">
       <c r="A394" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B394" t="inlineStr">
@@ -11472,7 +11472,7 @@
     <row r="395">
       <c r="A395" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B395" t="inlineStr">
@@ -11500,7 +11500,7 @@
     <row r="396">
       <c r="A396" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B396" t="inlineStr">
@@ -11528,7 +11528,7 @@
     <row r="397">
       <c r="A397" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B397" t="inlineStr">
@@ -11556,7 +11556,7 @@
     <row r="398">
       <c r="A398" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B398" t="inlineStr">
@@ -11584,7 +11584,7 @@
     <row r="399">
       <c r="A399" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B399" t="inlineStr">
@@ -11612,7 +11612,7 @@
     <row r="400">
       <c r="A400" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B400" t="inlineStr">
@@ -11640,7 +11640,7 @@
     <row r="401">
       <c r="A401" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B401" t="inlineStr">
@@ -11668,7 +11668,7 @@
     <row r="402">
       <c r="A402" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B402" t="inlineStr">
@@ -11696,7 +11696,7 @@
     <row r="403">
       <c r="A403" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B403" t="inlineStr">
@@ -11724,7 +11724,7 @@
     <row r="404">
       <c r="A404" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B404" t="inlineStr">
@@ -11746,13 +11746,13 @@
         <v>1</v>
       </c>
       <c r="F404" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="405">
       <c r="A405" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B405" t="inlineStr">
@@ -11780,7 +11780,7 @@
     <row r="406">
       <c r="A406" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B406" t="inlineStr">
@@ -11808,7 +11808,7 @@
     <row r="407">
       <c r="A407" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B407" t="inlineStr">
@@ -11836,7 +11836,7 @@
     <row r="408">
       <c r="A408" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B408" t="inlineStr">
@@ -11864,7 +11864,7 @@
     <row r="409">
       <c r="A409" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B409" t="inlineStr">
@@ -11892,7 +11892,7 @@
     <row r="410">
       <c r="A410" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B410" t="inlineStr">
@@ -11920,7 +11920,7 @@
     <row r="411">
       <c r="A411" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B411" t="inlineStr">
@@ -11948,7 +11948,7 @@
     <row r="412">
       <c r="A412" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B412" t="inlineStr">
@@ -11976,7 +11976,7 @@
     <row r="413">
       <c r="A413" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B413" t="inlineStr">
@@ -12004,7 +12004,7 @@
     <row r="414">
       <c r="A414" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B414" t="inlineStr">
@@ -12032,7 +12032,7 @@
     <row r="415">
       <c r="A415" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B415" t="inlineStr">
@@ -12060,7 +12060,7 @@
     <row r="416">
       <c r="A416" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B416" t="inlineStr">
@@ -12088,7 +12088,7 @@
     <row r="417">
       <c r="A417" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B417" t="inlineStr">
@@ -12116,7 +12116,7 @@
     <row r="418">
       <c r="A418" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B418" t="inlineStr">
@@ -12144,7 +12144,7 @@
     <row r="419">
       <c r="A419" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B419" t="inlineStr">
@@ -12172,7 +12172,7 @@
     <row r="420">
       <c r="A420" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B420" t="inlineStr">
@@ -12200,7 +12200,7 @@
     <row r="421">
       <c r="A421" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B421" t="inlineStr">
@@ -12228,7 +12228,7 @@
     <row r="422">
       <c r="A422" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B422" t="inlineStr">
@@ -12256,7 +12256,7 @@
     <row r="423">
       <c r="A423" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B423" t="inlineStr">
@@ -12284,7 +12284,7 @@
     <row r="424">
       <c r="A424" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B424" t="inlineStr">
@@ -12312,7 +12312,7 @@
     <row r="425">
       <c r="A425" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B425" t="inlineStr">
@@ -12340,7 +12340,7 @@
     <row r="426">
       <c r="A426" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B426" t="inlineStr">
@@ -12368,7 +12368,7 @@
     <row r="427">
       <c r="A427" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B427" t="inlineStr">
@@ -12390,13 +12390,13 @@
         <v>1</v>
       </c>
       <c r="F427" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="428">
       <c r="A428" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B428" t="inlineStr">
@@ -12424,7 +12424,7 @@
     <row r="429">
       <c r="A429" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B429" t="inlineStr">
@@ -12452,7 +12452,7 @@
     <row r="430">
       <c r="A430" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B430" t="inlineStr">
@@ -12480,7 +12480,7 @@
     <row r="431">
       <c r="A431" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B431" t="inlineStr">
@@ -12508,7 +12508,7 @@
     <row r="432">
       <c r="A432" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B432" t="inlineStr">
@@ -12536,7 +12536,7 @@
     <row r="433">
       <c r="A433" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B433" t="inlineStr">
@@ -12564,7 +12564,7 @@
     <row r="434">
       <c r="A434" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B434" t="inlineStr">
@@ -12592,7 +12592,7 @@
     <row r="435">
       <c r="A435" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B435" t="inlineStr">
@@ -12620,7 +12620,7 @@
     <row r="436">
       <c r="A436" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B436" t="inlineStr">
@@ -12648,7 +12648,7 @@
     <row r="437">
       <c r="A437" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B437" t="inlineStr">
@@ -12676,7 +12676,7 @@
     <row r="438">
       <c r="A438" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B438" t="inlineStr">
@@ -12704,7 +12704,7 @@
     <row r="439">
       <c r="A439" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B439" t="inlineStr">
@@ -12732,7 +12732,7 @@
     <row r="440">
       <c r="A440" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B440" t="inlineStr">
@@ -12760,7 +12760,7 @@
     <row r="441">
       <c r="A441" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B441" t="inlineStr">
@@ -12788,7 +12788,7 @@
     <row r="442">
       <c r="A442" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B442" t="inlineStr">
@@ -12816,7 +12816,7 @@
     <row r="443">
       <c r="A443" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B443" t="inlineStr">
@@ -12844,7 +12844,7 @@
     <row r="444">
       <c r="A444" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B444" t="inlineStr">
@@ -12872,7 +12872,7 @@
     <row r="445">
       <c r="A445" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B445" t="inlineStr">
@@ -12900,7 +12900,7 @@
     <row r="446">
       <c r="A446" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B446" t="inlineStr">
@@ -12928,7 +12928,7 @@
     <row r="447">
       <c r="A447" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B447" t="inlineStr">
@@ -12956,7 +12956,7 @@
     <row r="448">
       <c r="A448" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B448" t="inlineStr">
@@ -12984,7 +12984,7 @@
     <row r="449">
       <c r="A449" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B449" t="inlineStr">
@@ -13012,7 +13012,7 @@
     <row r="450">
       <c r="A450" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B450" t="inlineStr">
@@ -13040,7 +13040,7 @@
     <row r="451">
       <c r="A451" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B451" t="inlineStr">
@@ -13068,7 +13068,7 @@
     <row r="452">
       <c r="A452" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B452" t="inlineStr">
@@ -13096,7 +13096,7 @@
     <row r="453">
       <c r="A453" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B453" t="inlineStr">
@@ -13124,7 +13124,7 @@
     <row r="454">
       <c r="A454" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B454" t="inlineStr">
@@ -13152,7 +13152,7 @@
     <row r="455">
       <c r="A455" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B455" t="inlineStr">
@@ -13180,7 +13180,7 @@
     <row r="456">
       <c r="A456" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B456" t="inlineStr">
@@ -13208,7 +13208,7 @@
     <row r="457">
       <c r="A457" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B457" t="inlineStr">
@@ -13236,7 +13236,7 @@
     <row r="458">
       <c r="A458" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B458" t="inlineStr">
@@ -13264,7 +13264,7 @@
     <row r="459">
       <c r="A459" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B459" t="inlineStr">
@@ -13292,7 +13292,7 @@
     <row r="460">
       <c r="A460" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B460" t="inlineStr">
@@ -13320,7 +13320,7 @@
     <row r="461">
       <c r="A461" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B461" t="inlineStr">
@@ -13348,7 +13348,7 @@
     <row r="462">
       <c r="A462" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B462" t="inlineStr">
@@ -13376,7 +13376,7 @@
     <row r="463">
       <c r="A463" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B463" t="inlineStr">
@@ -13404,7 +13404,7 @@
     <row r="464">
       <c r="A464" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B464" t="inlineStr">
@@ -13432,7 +13432,7 @@
     <row r="465">
       <c r="A465" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B465" t="inlineStr">
@@ -13460,7 +13460,7 @@
     <row r="466">
       <c r="A466" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B466" t="inlineStr">
@@ -13488,7 +13488,7 @@
     <row r="467">
       <c r="A467" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B467" t="inlineStr">
@@ -13516,7 +13516,7 @@
     <row r="468">
       <c r="A468" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B468" t="inlineStr">
@@ -13544,7 +13544,7 @@
     <row r="469">
       <c r="A469" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B469" t="inlineStr">
@@ -13572,7 +13572,7 @@
     <row r="470">
       <c r="A470" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B470" t="inlineStr">
@@ -13600,7 +13600,7 @@
     <row r="471">
       <c r="A471" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B471" t="inlineStr">
@@ -13628,7 +13628,7 @@
     <row r="472">
       <c r="A472" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B472" t="inlineStr">
@@ -13656,7 +13656,7 @@
     <row r="473">
       <c r="A473" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B473" t="inlineStr">
@@ -13684,7 +13684,7 @@
     <row r="474">
       <c r="A474" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B474" t="inlineStr">
@@ -13712,7 +13712,7 @@
     <row r="475">
       <c r="A475" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B475" t="inlineStr">
@@ -13740,7 +13740,7 @@
     <row r="476">
       <c r="A476" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B476" t="inlineStr">
@@ -13768,7 +13768,7 @@
     <row r="477">
       <c r="A477" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B477" t="inlineStr">
@@ -13796,7 +13796,7 @@
     <row r="478">
       <c r="A478" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B478" t="inlineStr">
@@ -13824,7 +13824,7 @@
     <row r="479">
       <c r="A479" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B479" t="inlineStr">
@@ -13852,7 +13852,7 @@
     <row r="480">
       <c r="A480" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B480" t="inlineStr">
@@ -13880,7 +13880,7 @@
     <row r="481">
       <c r="A481" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B481" t="inlineStr">
@@ -13908,7 +13908,7 @@
     <row r="482">
       <c r="A482" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B482" t="inlineStr">
@@ -13936,7 +13936,7 @@
     <row r="483">
       <c r="A483" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B483" t="inlineStr">
@@ -13964,7 +13964,7 @@
     <row r="484">
       <c r="A484" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B484" t="inlineStr">
@@ -13992,7 +13992,7 @@
     <row r="485">
       <c r="A485" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B485" t="inlineStr">
@@ -14020,7 +14020,7 @@
     <row r="486">
       <c r="A486" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B486" t="inlineStr">
@@ -14048,7 +14048,7 @@
     <row r="487">
       <c r="A487" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B487" t="inlineStr">
@@ -14076,7 +14076,7 @@
     <row r="488">
       <c r="A488" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B488" t="inlineStr">
@@ -14104,7 +14104,7 @@
     <row r="489">
       <c r="A489" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B489" t="inlineStr">
@@ -14132,7 +14132,7 @@
     <row r="490">
       <c r="A490" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B490" t="inlineStr">
@@ -14160,7 +14160,7 @@
     <row r="491">
       <c r="A491" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B491" t="inlineStr">
@@ -14188,7 +14188,7 @@
     <row r="492">
       <c r="A492" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B492" t="inlineStr">
@@ -14216,7 +14216,7 @@
     <row r="493">
       <c r="A493" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B493" t="inlineStr">
@@ -14244,7 +14244,7 @@
     <row r="494">
       <c r="A494" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B494" t="inlineStr">
@@ -14272,7 +14272,7 @@
     <row r="495">
       <c r="A495" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B495" t="inlineStr">
@@ -14300,7 +14300,7 @@
     <row r="496">
       <c r="A496" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B496" t="inlineStr">
@@ -14328,7 +14328,7 @@
     <row r="497">
       <c r="A497" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B497" t="inlineStr">
@@ -14356,7 +14356,7 @@
     <row r="498">
       <c r="A498" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B498" t="inlineStr">
@@ -14384,7 +14384,7 @@
     <row r="499">
       <c r="A499" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B499" t="inlineStr">
@@ -14412,7 +14412,7 @@
     <row r="500">
       <c r="A500" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B500" t="inlineStr">
@@ -14440,7 +14440,7 @@
     <row r="501">
       <c r="A501" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B501" t="inlineStr">
@@ -14468,7 +14468,7 @@
     <row r="502">
       <c r="A502" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B502" t="inlineStr">
@@ -14496,7 +14496,7 @@
     <row r="503">
       <c r="A503" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B503" t="inlineStr">
@@ -14524,7 +14524,7 @@
     <row r="504">
       <c r="A504" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B504" t="inlineStr">
@@ -14552,7 +14552,7 @@
     <row r="505">
       <c r="A505" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B505" t="inlineStr">
@@ -14580,7 +14580,7 @@
     <row r="506">
       <c r="A506" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B506" t="inlineStr">
@@ -14608,7 +14608,7 @@
     <row r="507">
       <c r="A507" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B507" t="inlineStr">
@@ -14636,7 +14636,7 @@
     <row r="508">
       <c r="A508" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B508" t="inlineStr">
@@ -14664,7 +14664,7 @@
     <row r="509">
       <c r="A509" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B509" t="inlineStr">
@@ -14692,7 +14692,7 @@
     <row r="510">
       <c r="A510" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B510" t="inlineStr">
@@ -14720,7 +14720,7 @@
     <row r="511">
       <c r="A511" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B511" t="inlineStr">
@@ -14748,7 +14748,7 @@
     <row r="512">
       <c r="A512" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B512" t="inlineStr">
@@ -14776,7 +14776,7 @@
     <row r="513">
       <c r="A513" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B513" t="inlineStr">
@@ -14804,7 +14804,7 @@
     <row r="514">
       <c r="A514" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B514" t="inlineStr">
@@ -14832,7 +14832,7 @@
     <row r="515">
       <c r="A515" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B515" t="inlineStr">
@@ -14860,7 +14860,7 @@
     <row r="516">
       <c r="A516" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B516" t="inlineStr">
@@ -14888,7 +14888,7 @@
     <row r="517">
       <c r="A517" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B517" t="inlineStr">
@@ -14916,7 +14916,7 @@
     <row r="518">
       <c r="A518" t="inlineStr">
         <is>
-          <t>2025-07-25 12:21:09</t>
+          <t>2025-07-25 13:48:50</t>
         </is>
       </c>
       <c r="B518" t="inlineStr">

</xml_diff>

<commit_message>
Atualização automática [Fri Jul 25 14:14:34 UTC 2025]
</commit_message>
<xml_diff>
--- a/livelo_parceiros.xlsx
+++ b/livelo_parceiros.xlsx
@@ -7720,7 +7720,7 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
@@ -7748,7 +7748,7 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
@@ -7776,7 +7776,7 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
@@ -7804,7 +7804,7 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
@@ -7832,7 +7832,7 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
@@ -7860,7 +7860,7 @@
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
@@ -7888,7 +7888,7 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
@@ -7916,7 +7916,7 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
@@ -7944,7 +7944,7 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
@@ -7972,7 +7972,7 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
@@ -8000,7 +8000,7 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
@@ -8028,7 +8028,7 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
@@ -8056,7 +8056,7 @@
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
@@ -8084,7 +8084,7 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
@@ -8112,7 +8112,7 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
@@ -8140,7 +8140,7 @@
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
@@ -8168,7 +8168,7 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
@@ -8196,7 +8196,7 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
@@ -8224,7 +8224,7 @@
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
@@ -8252,7 +8252,7 @@
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
@@ -8280,7 +8280,7 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
@@ -8308,7 +8308,7 @@
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
@@ -8336,7 +8336,7 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
@@ -8364,7 +8364,7 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
@@ -8392,7 +8392,7 @@
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
@@ -8420,7 +8420,7 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
@@ -8448,7 +8448,7 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
@@ -8476,7 +8476,7 @@
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
@@ -8504,7 +8504,7 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
@@ -8532,7 +8532,7 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
@@ -8560,7 +8560,7 @@
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
@@ -8588,7 +8588,7 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
@@ -8616,7 +8616,7 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
@@ -8644,7 +8644,7 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
@@ -8672,7 +8672,7 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
@@ -8700,7 +8700,7 @@
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
@@ -8728,7 +8728,7 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
@@ -8756,7 +8756,7 @@
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
@@ -8784,7 +8784,7 @@
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
@@ -8812,7 +8812,7 @@
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
@@ -8840,7 +8840,7 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
@@ -8868,7 +8868,7 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
@@ -8896,7 +8896,7 @@
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
@@ -8924,7 +8924,7 @@
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
@@ -8952,7 +8952,7 @@
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
@@ -8980,7 +8980,7 @@
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
@@ -9008,7 +9008,7 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
@@ -9036,7 +9036,7 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
@@ -9064,7 +9064,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
@@ -9092,7 +9092,7 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
@@ -9120,7 +9120,7 @@
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
@@ -9148,7 +9148,7 @@
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
@@ -9176,7 +9176,7 @@
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
@@ -9204,7 +9204,7 @@
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
@@ -9232,7 +9232,7 @@
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
@@ -9260,7 +9260,7 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
@@ -9288,7 +9288,7 @@
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
@@ -9316,7 +9316,7 @@
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
@@ -9344,7 +9344,7 @@
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
@@ -9372,7 +9372,7 @@
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
@@ -9400,7 +9400,7 @@
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
@@ -9428,7 +9428,7 @@
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
@@ -9456,7 +9456,7 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
@@ -9484,7 +9484,7 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
@@ -9512,7 +9512,7 @@
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
@@ -9540,7 +9540,7 @@
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
@@ -9568,7 +9568,7 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
@@ -9596,7 +9596,7 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
@@ -9624,7 +9624,7 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
@@ -9652,7 +9652,7 @@
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
@@ -9680,7 +9680,7 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
@@ -9708,7 +9708,7 @@
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
@@ -9736,7 +9736,7 @@
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B333" t="inlineStr">
@@ -9764,7 +9764,7 @@
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B334" t="inlineStr">
@@ -9792,7 +9792,7 @@
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B335" t="inlineStr">
@@ -9820,7 +9820,7 @@
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B336" t="inlineStr">
@@ -9848,7 +9848,7 @@
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B337" t="inlineStr">
@@ -9876,7 +9876,7 @@
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B338" t="inlineStr">
@@ -9904,7 +9904,7 @@
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B339" t="inlineStr">
@@ -9932,7 +9932,7 @@
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B340" t="inlineStr">
@@ -9960,7 +9960,7 @@
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B341" t="inlineStr">
@@ -9988,7 +9988,7 @@
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B342" t="inlineStr">
@@ -10016,7 +10016,7 @@
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B343" t="inlineStr">
@@ -10044,7 +10044,7 @@
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B344" t="inlineStr">
@@ -10072,7 +10072,7 @@
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B345" t="inlineStr">
@@ -10100,7 +10100,7 @@
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B346" t="inlineStr">
@@ -10128,7 +10128,7 @@
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B347" t="inlineStr">
@@ -10156,7 +10156,7 @@
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B348" t="inlineStr">
@@ -10184,7 +10184,7 @@
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B349" t="inlineStr">
@@ -10212,7 +10212,7 @@
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B350" t="inlineStr">
@@ -10240,7 +10240,7 @@
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B351" t="inlineStr">
@@ -10268,7 +10268,7 @@
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B352" t="inlineStr">
@@ -10296,7 +10296,7 @@
     <row r="353">
       <c r="A353" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B353" t="inlineStr">
@@ -10324,7 +10324,7 @@
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B354" t="inlineStr">
@@ -10352,7 +10352,7 @@
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B355" t="inlineStr">
@@ -10380,7 +10380,7 @@
     <row r="356">
       <c r="A356" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B356" t="inlineStr">
@@ -10408,7 +10408,7 @@
     <row r="357">
       <c r="A357" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B357" t="inlineStr">
@@ -10436,7 +10436,7 @@
     <row r="358">
       <c r="A358" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B358" t="inlineStr">
@@ -10464,7 +10464,7 @@
     <row r="359">
       <c r="A359" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B359" t="inlineStr">
@@ -10492,7 +10492,7 @@
     <row r="360">
       <c r="A360" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B360" t="inlineStr">
@@ -10520,7 +10520,7 @@
     <row r="361">
       <c r="A361" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B361" t="inlineStr">
@@ -10548,7 +10548,7 @@
     <row r="362">
       <c r="A362" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B362" t="inlineStr">
@@ -10576,7 +10576,7 @@
     <row r="363">
       <c r="A363" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B363" t="inlineStr">
@@ -10604,7 +10604,7 @@
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B364" t="inlineStr">
@@ -10632,7 +10632,7 @@
     <row r="365">
       <c r="A365" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B365" t="inlineStr">
@@ -10660,7 +10660,7 @@
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B366" t="inlineStr">
@@ -10688,7 +10688,7 @@
     <row r="367">
       <c r="A367" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B367" t="inlineStr">
@@ -10716,7 +10716,7 @@
     <row r="368">
       <c r="A368" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B368" t="inlineStr">
@@ -10744,7 +10744,7 @@
     <row r="369">
       <c r="A369" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B369" t="inlineStr">
@@ -10772,7 +10772,7 @@
     <row r="370">
       <c r="A370" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B370" t="inlineStr">
@@ -10800,7 +10800,7 @@
     <row r="371">
       <c r="A371" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B371" t="inlineStr">
@@ -10828,7 +10828,7 @@
     <row r="372">
       <c r="A372" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B372" t="inlineStr">
@@ -10856,7 +10856,7 @@
     <row r="373">
       <c r="A373" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B373" t="inlineStr">
@@ -10884,7 +10884,7 @@
     <row r="374">
       <c r="A374" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B374" t="inlineStr">
@@ -10912,7 +10912,7 @@
     <row r="375">
       <c r="A375" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B375" t="inlineStr">
@@ -10940,7 +10940,7 @@
     <row r="376">
       <c r="A376" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B376" t="inlineStr">
@@ -10968,7 +10968,7 @@
     <row r="377">
       <c r="A377" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B377" t="inlineStr">
@@ -10996,7 +10996,7 @@
     <row r="378">
       <c r="A378" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B378" t="inlineStr">
@@ -11024,7 +11024,7 @@
     <row r="379">
       <c r="A379" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B379" t="inlineStr">
@@ -11052,7 +11052,7 @@
     <row r="380">
       <c r="A380" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B380" t="inlineStr">
@@ -11080,7 +11080,7 @@
     <row r="381">
       <c r="A381" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B381" t="inlineStr">
@@ -11108,7 +11108,7 @@
     <row r="382">
       <c r="A382" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B382" t="inlineStr">
@@ -11136,7 +11136,7 @@
     <row r="383">
       <c r="A383" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B383" t="inlineStr">
@@ -11164,7 +11164,7 @@
     <row r="384">
       <c r="A384" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B384" t="inlineStr">
@@ -11192,7 +11192,7 @@
     <row r="385">
       <c r="A385" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B385" t="inlineStr">
@@ -11220,7 +11220,7 @@
     <row r="386">
       <c r="A386" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B386" t="inlineStr">
@@ -11248,7 +11248,7 @@
     <row r="387">
       <c r="A387" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B387" t="inlineStr">
@@ -11276,7 +11276,7 @@
     <row r="388">
       <c r="A388" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B388" t="inlineStr">
@@ -11304,7 +11304,7 @@
     <row r="389">
       <c r="A389" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B389" t="inlineStr">
@@ -11332,7 +11332,7 @@
     <row r="390">
       <c r="A390" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B390" t="inlineStr">
@@ -11360,7 +11360,7 @@
     <row r="391">
       <c r="A391" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B391" t="inlineStr">
@@ -11388,7 +11388,7 @@
     <row r="392">
       <c r="A392" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B392" t="inlineStr">
@@ -11416,7 +11416,7 @@
     <row r="393">
       <c r="A393" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B393" t="inlineStr">
@@ -11444,7 +11444,7 @@
     <row r="394">
       <c r="A394" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B394" t="inlineStr">
@@ -11472,7 +11472,7 @@
     <row r="395">
       <c r="A395" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B395" t="inlineStr">
@@ -11500,7 +11500,7 @@
     <row r="396">
       <c r="A396" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B396" t="inlineStr">
@@ -11528,7 +11528,7 @@
     <row r="397">
       <c r="A397" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B397" t="inlineStr">
@@ -11556,7 +11556,7 @@
     <row r="398">
       <c r="A398" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B398" t="inlineStr">
@@ -11584,7 +11584,7 @@
     <row r="399">
       <c r="A399" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B399" t="inlineStr">
@@ -11612,7 +11612,7 @@
     <row r="400">
       <c r="A400" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B400" t="inlineStr">
@@ -11640,7 +11640,7 @@
     <row r="401">
       <c r="A401" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B401" t="inlineStr">
@@ -11668,7 +11668,7 @@
     <row r="402">
       <c r="A402" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B402" t="inlineStr">
@@ -11696,7 +11696,7 @@
     <row r="403">
       <c r="A403" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B403" t="inlineStr">
@@ -11724,7 +11724,7 @@
     <row r="404">
       <c r="A404" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B404" t="inlineStr">
@@ -11752,7 +11752,7 @@
     <row r="405">
       <c r="A405" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B405" t="inlineStr">
@@ -11780,7 +11780,7 @@
     <row r="406">
       <c r="A406" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B406" t="inlineStr">
@@ -11808,7 +11808,7 @@
     <row r="407">
       <c r="A407" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B407" t="inlineStr">
@@ -11836,7 +11836,7 @@
     <row r="408">
       <c r="A408" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B408" t="inlineStr">
@@ -11864,7 +11864,7 @@
     <row r="409">
       <c r="A409" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B409" t="inlineStr">
@@ -11892,7 +11892,7 @@
     <row r="410">
       <c r="A410" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B410" t="inlineStr">
@@ -11920,7 +11920,7 @@
     <row r="411">
       <c r="A411" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B411" t="inlineStr">
@@ -11948,7 +11948,7 @@
     <row r="412">
       <c r="A412" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B412" t="inlineStr">
@@ -11976,7 +11976,7 @@
     <row r="413">
       <c r="A413" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B413" t="inlineStr">
@@ -12004,7 +12004,7 @@
     <row r="414">
       <c r="A414" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B414" t="inlineStr">
@@ -12032,7 +12032,7 @@
     <row r="415">
       <c r="A415" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B415" t="inlineStr">
@@ -12060,7 +12060,7 @@
     <row r="416">
       <c r="A416" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B416" t="inlineStr">
@@ -12088,7 +12088,7 @@
     <row r="417">
       <c r="A417" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B417" t="inlineStr">
@@ -12116,7 +12116,7 @@
     <row r="418">
       <c r="A418" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B418" t="inlineStr">
@@ -12144,7 +12144,7 @@
     <row r="419">
       <c r="A419" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B419" t="inlineStr">
@@ -12172,7 +12172,7 @@
     <row r="420">
       <c r="A420" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B420" t="inlineStr">
@@ -12200,7 +12200,7 @@
     <row r="421">
       <c r="A421" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B421" t="inlineStr">
@@ -12228,7 +12228,7 @@
     <row r="422">
       <c r="A422" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B422" t="inlineStr">
@@ -12256,7 +12256,7 @@
     <row r="423">
       <c r="A423" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B423" t="inlineStr">
@@ -12284,7 +12284,7 @@
     <row r="424">
       <c r="A424" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B424" t="inlineStr">
@@ -12312,7 +12312,7 @@
     <row r="425">
       <c r="A425" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B425" t="inlineStr">
@@ -12340,7 +12340,7 @@
     <row r="426">
       <c r="A426" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B426" t="inlineStr">
@@ -12368,7 +12368,7 @@
     <row r="427">
       <c r="A427" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B427" t="inlineStr">
@@ -12396,7 +12396,7 @@
     <row r="428">
       <c r="A428" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B428" t="inlineStr">
@@ -12424,7 +12424,7 @@
     <row r="429">
       <c r="A429" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B429" t="inlineStr">
@@ -12452,7 +12452,7 @@
     <row r="430">
       <c r="A430" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B430" t="inlineStr">
@@ -12480,7 +12480,7 @@
     <row r="431">
       <c r="A431" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B431" t="inlineStr">
@@ -12508,7 +12508,7 @@
     <row r="432">
       <c r="A432" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B432" t="inlineStr">
@@ -12536,7 +12536,7 @@
     <row r="433">
       <c r="A433" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B433" t="inlineStr">
@@ -12564,7 +12564,7 @@
     <row r="434">
       <c r="A434" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B434" t="inlineStr">
@@ -12592,7 +12592,7 @@
     <row r="435">
       <c r="A435" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B435" t="inlineStr">
@@ -12620,7 +12620,7 @@
     <row r="436">
       <c r="A436" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B436" t="inlineStr">
@@ -12648,7 +12648,7 @@
     <row r="437">
       <c r="A437" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B437" t="inlineStr">
@@ -12676,7 +12676,7 @@
     <row r="438">
       <c r="A438" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B438" t="inlineStr">
@@ -12704,7 +12704,7 @@
     <row r="439">
       <c r="A439" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B439" t="inlineStr">
@@ -12732,7 +12732,7 @@
     <row r="440">
       <c r="A440" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B440" t="inlineStr">
@@ -12760,7 +12760,7 @@
     <row r="441">
       <c r="A441" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B441" t="inlineStr">
@@ -12788,7 +12788,7 @@
     <row r="442">
       <c r="A442" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B442" t="inlineStr">
@@ -12816,7 +12816,7 @@
     <row r="443">
       <c r="A443" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B443" t="inlineStr">
@@ -12844,7 +12844,7 @@
     <row r="444">
       <c r="A444" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B444" t="inlineStr">
@@ -12872,7 +12872,7 @@
     <row r="445">
       <c r="A445" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B445" t="inlineStr">
@@ -12900,7 +12900,7 @@
     <row r="446">
       <c r="A446" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B446" t="inlineStr">
@@ -12928,7 +12928,7 @@
     <row r="447">
       <c r="A447" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B447" t="inlineStr">
@@ -12956,7 +12956,7 @@
     <row r="448">
       <c r="A448" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B448" t="inlineStr">
@@ -12984,7 +12984,7 @@
     <row r="449">
       <c r="A449" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B449" t="inlineStr">
@@ -13012,7 +13012,7 @@
     <row r="450">
       <c r="A450" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B450" t="inlineStr">
@@ -13040,7 +13040,7 @@
     <row r="451">
       <c r="A451" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B451" t="inlineStr">
@@ -13068,7 +13068,7 @@
     <row r="452">
       <c r="A452" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B452" t="inlineStr">
@@ -13096,7 +13096,7 @@
     <row r="453">
       <c r="A453" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B453" t="inlineStr">
@@ -13124,7 +13124,7 @@
     <row r="454">
       <c r="A454" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B454" t="inlineStr">
@@ -13152,7 +13152,7 @@
     <row r="455">
       <c r="A455" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B455" t="inlineStr">
@@ -13180,7 +13180,7 @@
     <row r="456">
       <c r="A456" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B456" t="inlineStr">
@@ -13208,7 +13208,7 @@
     <row r="457">
       <c r="A457" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B457" t="inlineStr">
@@ -13236,7 +13236,7 @@
     <row r="458">
       <c r="A458" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B458" t="inlineStr">
@@ -13264,7 +13264,7 @@
     <row r="459">
       <c r="A459" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B459" t="inlineStr">
@@ -13292,7 +13292,7 @@
     <row r="460">
       <c r="A460" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B460" t="inlineStr">
@@ -13320,7 +13320,7 @@
     <row r="461">
       <c r="A461" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B461" t="inlineStr">
@@ -13348,7 +13348,7 @@
     <row r="462">
       <c r="A462" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B462" t="inlineStr">
@@ -13376,7 +13376,7 @@
     <row r="463">
       <c r="A463" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B463" t="inlineStr">
@@ -13404,7 +13404,7 @@
     <row r="464">
       <c r="A464" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B464" t="inlineStr">
@@ -13432,7 +13432,7 @@
     <row r="465">
       <c r="A465" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B465" t="inlineStr">
@@ -13460,7 +13460,7 @@
     <row r="466">
       <c r="A466" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B466" t="inlineStr">
@@ -13488,7 +13488,7 @@
     <row r="467">
       <c r="A467" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B467" t="inlineStr">
@@ -13516,7 +13516,7 @@
     <row r="468">
       <c r="A468" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B468" t="inlineStr">
@@ -13544,7 +13544,7 @@
     <row r="469">
       <c r="A469" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B469" t="inlineStr">
@@ -13572,7 +13572,7 @@
     <row r="470">
       <c r="A470" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B470" t="inlineStr">
@@ -13600,7 +13600,7 @@
     <row r="471">
       <c r="A471" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B471" t="inlineStr">
@@ -13628,7 +13628,7 @@
     <row r="472">
       <c r="A472" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B472" t="inlineStr">
@@ -13656,7 +13656,7 @@
     <row r="473">
       <c r="A473" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B473" t="inlineStr">
@@ -13684,7 +13684,7 @@
     <row r="474">
       <c r="A474" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B474" t="inlineStr">
@@ -13712,7 +13712,7 @@
     <row r="475">
       <c r="A475" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B475" t="inlineStr">
@@ -13740,7 +13740,7 @@
     <row r="476">
       <c r="A476" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B476" t="inlineStr">
@@ -13768,7 +13768,7 @@
     <row r="477">
       <c r="A477" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B477" t="inlineStr">
@@ -13796,7 +13796,7 @@
     <row r="478">
       <c r="A478" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B478" t="inlineStr">
@@ -13824,7 +13824,7 @@
     <row r="479">
       <c r="A479" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B479" t="inlineStr">
@@ -13852,7 +13852,7 @@
     <row r="480">
       <c r="A480" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B480" t="inlineStr">
@@ -13880,7 +13880,7 @@
     <row r="481">
       <c r="A481" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B481" t="inlineStr">
@@ -13908,7 +13908,7 @@
     <row r="482">
       <c r="A482" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B482" t="inlineStr">
@@ -13936,7 +13936,7 @@
     <row r="483">
       <c r="A483" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B483" t="inlineStr">
@@ -13964,7 +13964,7 @@
     <row r="484">
       <c r="A484" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B484" t="inlineStr">
@@ -13992,7 +13992,7 @@
     <row r="485">
       <c r="A485" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B485" t="inlineStr">
@@ -14020,7 +14020,7 @@
     <row r="486">
       <c r="A486" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B486" t="inlineStr">
@@ -14048,7 +14048,7 @@
     <row r="487">
       <c r="A487" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B487" t="inlineStr">
@@ -14076,7 +14076,7 @@
     <row r="488">
       <c r="A488" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B488" t="inlineStr">
@@ -14104,7 +14104,7 @@
     <row r="489">
       <c r="A489" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B489" t="inlineStr">
@@ -14132,7 +14132,7 @@
     <row r="490">
       <c r="A490" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B490" t="inlineStr">
@@ -14160,7 +14160,7 @@
     <row r="491">
       <c r="A491" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B491" t="inlineStr">
@@ -14188,7 +14188,7 @@
     <row r="492">
       <c r="A492" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B492" t="inlineStr">
@@ -14216,7 +14216,7 @@
     <row r="493">
       <c r="A493" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B493" t="inlineStr">
@@ -14244,7 +14244,7 @@
     <row r="494">
       <c r="A494" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B494" t="inlineStr">
@@ -14272,7 +14272,7 @@
     <row r="495">
       <c r="A495" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B495" t="inlineStr">
@@ -14300,7 +14300,7 @@
     <row r="496">
       <c r="A496" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B496" t="inlineStr">
@@ -14328,7 +14328,7 @@
     <row r="497">
       <c r="A497" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B497" t="inlineStr">
@@ -14356,7 +14356,7 @@
     <row r="498">
       <c r="A498" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B498" t="inlineStr">
@@ -14384,7 +14384,7 @@
     <row r="499">
       <c r="A499" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B499" t="inlineStr">
@@ -14412,7 +14412,7 @@
     <row r="500">
       <c r="A500" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B500" t="inlineStr">
@@ -14440,7 +14440,7 @@
     <row r="501">
       <c r="A501" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B501" t="inlineStr">
@@ -14468,7 +14468,7 @@
     <row r="502">
       <c r="A502" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B502" t="inlineStr">
@@ -14496,7 +14496,7 @@
     <row r="503">
       <c r="A503" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B503" t="inlineStr">
@@ -14524,7 +14524,7 @@
     <row r="504">
       <c r="A504" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B504" t="inlineStr">
@@ -14552,7 +14552,7 @@
     <row r="505">
       <c r="A505" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B505" t="inlineStr">
@@ -14580,7 +14580,7 @@
     <row r="506">
       <c r="A506" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B506" t="inlineStr">
@@ -14608,7 +14608,7 @@
     <row r="507">
       <c r="A507" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B507" t="inlineStr">
@@ -14636,7 +14636,7 @@
     <row r="508">
       <c r="A508" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B508" t="inlineStr">
@@ -14664,7 +14664,7 @@
     <row r="509">
       <c r="A509" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B509" t="inlineStr">
@@ -14692,7 +14692,7 @@
     <row r="510">
       <c r="A510" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B510" t="inlineStr">
@@ -14720,7 +14720,7 @@
     <row r="511">
       <c r="A511" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B511" t="inlineStr">
@@ -14748,7 +14748,7 @@
     <row r="512">
       <c r="A512" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B512" t="inlineStr">
@@ -14776,7 +14776,7 @@
     <row r="513">
       <c r="A513" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B513" t="inlineStr">
@@ -14804,7 +14804,7 @@
     <row r="514">
       <c r="A514" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B514" t="inlineStr">
@@ -14832,7 +14832,7 @@
     <row r="515">
       <c r="A515" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B515" t="inlineStr">
@@ -14860,7 +14860,7 @@
     <row r="516">
       <c r="A516" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B516" t="inlineStr">
@@ -14888,7 +14888,7 @@
     <row r="517">
       <c r="A517" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B517" t="inlineStr">
@@ -14916,7 +14916,7 @@
     <row r="518">
       <c r="A518" t="inlineStr">
         <is>
-          <t>2025-07-25 13:48:50</t>
+          <t>2025-07-25 14:14:09</t>
         </is>
       </c>
       <c r="B518" t="inlineStr">

</xml_diff>